<commit_message>
Finished most of dndClass and added MathUtils class
</commit_message>
<xml_diff>
--- a/classes/cleric/DivineDomains.xlsx
+++ b/classes/cleric/DivineDomains.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Ambition Domain</t>
   </si>
@@ -19,67 +19,25 @@
     <t>Arcana Domain</t>
   </si>
   <si>
-    <t>Blood Domain</t>
-  </si>
-  <si>
-    <t>City Domain</t>
-  </si>
-  <si>
-    <t>Death Domain</t>
-  </si>
-  <si>
-    <t>Forge Domain</t>
-  </si>
-  <si>
-    <t>Grave Domain</t>
-  </si>
-  <si>
-    <t>Knowledge Domain</t>
-  </si>
-  <si>
-    <t>Life Domain</t>
-  </si>
-  <si>
-    <t>Light Domain</t>
-  </si>
-  <si>
-    <t>Mind Domain</t>
-  </si>
-  <si>
-    <t>Nature Domain</t>
-  </si>
-  <si>
-    <t>Order Domain</t>
-  </si>
-  <si>
-    <t>Peace Domain</t>
-  </si>
-  <si>
-    <t>Protection Domain</t>
-  </si>
-  <si>
-    <t>Solidarity Domain</t>
-  </si>
-  <si>
-    <t>Strength Domain</t>
-  </si>
-  <si>
-    <t>Tempest Domain</t>
-  </si>
-  <si>
-    <t>Trickery Domain</t>
-  </si>
-  <si>
-    <t>Twilight Domain</t>
-  </si>
-  <si>
-    <t>Unity Domain</t>
-  </si>
-  <si>
-    <t>War Domain</t>
-  </si>
-  <si>
-    <t>Zeal Domain</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Arcana</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsAmbitionDomain.xlsx</t>
+  </si>
+  <si>
+    <t>true=classes/cleric/domains/BonusSpellsArcaneDomain.xlsx</t>
+  </si>
+  <si>
+    <t>false=</t>
+  </si>
+  <si>
+    <t>1/Warding Flare=2/Channel Divinity: Invoke Duplicity=6/Channel Divinity: Cloak of Shadows=8/Potent Spellcasting=17/Improved Duplicity</t>
+  </si>
+  <si>
+    <t>2/Channel Divinity: Arcane Abjuration=6/Spell Breaker=8/Potent Spellcasting</t>
   </si>
 </sst>
 </file>
@@ -343,68 +301,61 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>